<commit_message>
Update output data files
</commit_message>
<xml_diff>
--- a/output/not-graded/method-hybrid-results.xlsx
+++ b/output/not-graded/method-hybrid-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbutl20/PyCharmProjects/nlp-bnf-atc-mapping/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbutl20/PyCharmProjects/nlp-bnf-atc-mapping/output/not-graded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40090CFB-FB52-2840-BC03-96E89D4E78D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0569A3A9-376E-EE45-804D-E4B367D442E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21900" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="600" windowWidth="37980" windowHeight="20380" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Levenshtein Monge-Elkan" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11991" uniqueCount="3349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11992" uniqueCount="3350">
   <si>
     <t>bnf_chapter</t>
   </si>
@@ -10008,12 +10008,6 @@
     <t>Scorer</t>
   </si>
   <si>
-    <t>No Match</t>
-  </si>
-  <si>
-    <t>Match</t>
-  </si>
-  <si>
     <t>Num of Match</t>
   </si>
   <si>
@@ -10074,7 +10068,16 @@
     <t>Hit Rate</t>
   </si>
   <si>
-    <t>Adj Hit Rate</t>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>Adj. Rate</t>
+  </si>
+  <si>
+    <t>ROC</t>
   </si>
 </sst>
 </file>
@@ -10487,7 +10490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -16801,11 +16804,11 @@
         <v>1</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>1</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>4</v>
       </c>
     </row>
@@ -24161,11 +24164,11 @@
         <v>5</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>5</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>0</v>
       </c>
     </row>
@@ -31524,11 +31527,11 @@
         <v>5</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>5</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>0</v>
       </c>
     </row>
@@ -38881,11 +38884,11 @@
         <v>1</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>1</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>4</v>
       </c>
     </row>
@@ -46232,11 +46235,11 @@
         <v>1</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>1</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>4</v>
       </c>
     </row>
@@ -53622,11 +53625,11 @@
         <v>4</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>4</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>1</v>
       </c>
     </row>
@@ -61015,11 +61018,11 @@
         <v>5</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>5</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>0</v>
       </c>
     </row>
@@ -68369,11 +68372,11 @@
         <v>1</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N161" si="8">M130</f>
+        <f t="shared" ref="N130:N151" si="8">M130</f>
         <v>1</v>
       </c>
       <c r="Q130">
-        <f t="shared" ref="Q130:Q161" si="9">L130-SUM(N130:P130)</f>
+        <f t="shared" ref="Q130:Q151" si="9">L130-SUM(N130:P130)</f>
         <v>4</v>
       </c>
     </row>
@@ -69410,10 +69413,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -69435,59 +69438,62 @@
     <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3325</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3326</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3327</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3328</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3329</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3330</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3331</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3332</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>3333</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>3345</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>3336</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>3337</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>3347</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>3338</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>3348</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3339</v>
+        <v>3337</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" ca="1" si="0">COUNTBLANK(INDIRECT("'"&amp;A2&amp;"'!$K$2:$K$151"))</f>
@@ -69550,9 +69556,9 @@
         <v>0.88666666666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3340</v>
+        <v>3338</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
@@ -69615,9 +69621,9 @@
         <v>0.89333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3341</v>
+        <v>3339</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
@@ -69680,9 +69686,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3342</v>
+        <v>3340</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
@@ -69745,9 +69751,9 @@
         <v>0.88666666666666671</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3343</v>
+        <v>3341</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
@@ -69810,9 +69816,9 @@
         <v>0.87333333333333329</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3344</v>
+        <v>3342</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
@@ -69875,9 +69881,9 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3345</v>
+        <v>3343</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
@@ -69940,9 +69946,9 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3346</v>
+        <v>3344</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>

</xml_diff>